<commit_message>
Add last source code
</commit_message>
<xml_diff>
--- a/ui-testsuite/src/main/resources/TestData/ATR_AutoCanculated_Renewal.xlsx
+++ b/ui-testsuite/src/main/resources/TestData/ATR_AutoCanculated_Renewal.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="579">
   <si>
     <t>IB TYPE</t>
   </si>
@@ -1719,9 +1719,6 @@
     <t>move to Q3, cant reach eu</t>
   </si>
   <si>
-    <t>Underforecast</t>
-  </si>
-  <si>
     <t>Underforecast - FX Impact</t>
   </si>
   <si>
@@ -1737,9 +1734,6 @@
     <t>BOOKED</t>
   </si>
   <si>
-    <t>UPSELL</t>
-  </si>
-  <si>
     <t>No Response from Customer</t>
   </si>
   <si>
@@ -1749,9 +1743,6 @@
     <t>PO RECEIVED, pending credit approval. Upfront contracts payment delayed due to pending HP Vietnam to sign contract  1062 5897 2901</t>
   </si>
   <si>
-    <t>UNDER FORECAST</t>
-  </si>
-  <si>
     <t>pushing customer for PO this month, upside as since slow response by EU, last renewal happen in June only     BOM REVIEW BY EU, PARTIAL EOS, PENDING APPROVAL FOR UPGRADE</t>
   </si>
   <si>
@@ -1771,6 +1762,9 @@
   </si>
   <si>
     <t>EOT</t>
+  </si>
+  <si>
+    <t>Duplicate opportunity</t>
   </si>
 </sst>
 </file>
@@ -2588,8 +2582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FF10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="DL1" workbookViewId="0">
+      <selection activeCell="DV4" sqref="DV4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2713,9 +2707,9 @@
     <col min="123" max="123" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="124" max="124" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="125" max="125" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="127" max="127" width="59.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="129" max="129" width="29" style="1" bestFit="1" customWidth="1"/>
     <col min="130" max="130" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="131" max="131" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -2893,7 +2887,7 @@
         <v>45</v>
       </c>
       <c r="AU1" s="6" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="AV1" s="6" t="s">
         <v>46</v>
@@ -3551,11 +3545,8 @@
       <c r="DW2" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="DX2" s="1" t="s">
+      <c r="DY2" s="1" t="s">
         <v>563</v>
-      </c>
-      <c r="DY2" s="1" t="s">
-        <v>564</v>
       </c>
       <c r="DZ2" s="1">
         <f>DG2/EF2</f>
@@ -3917,7 +3908,7 @@
         <v>182</v>
       </c>
       <c r="DW3" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="DZ3" s="1">
         <f t="shared" ref="DZ3:DZ9" si="2">DG3/EF3</f>
@@ -3948,7 +3939,7 @@
       </c>
       <c r="EG3" s="1" t="str">
         <f t="shared" ref="EG3:EG9" ca="1" si="8" xml:space="preserve"> IF(AND(EI3="OPEN",DN3&lt;TODAY()),"OVERDUE","")</f>
-        <v/>
+        <v>OVERDUE</v>
       </c>
       <c r="EH3" s="21">
         <f t="shared" ref="EH3:EH6" si="9">EOMONTH(DN3,0)</f>
@@ -3988,13 +3979,13 @@
         <v>201</v>
       </c>
       <c r="EX3" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="EY3" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="EZ3" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="FD3" s="1" t="str">
         <f t="shared" ref="FD3:FD10" si="10" xml:space="preserve"> IF(FC3="","NO","YES")</f>
@@ -4311,6 +4302,9 @@
       <c r="DU4" s="1" t="s">
         <v>182</v>
       </c>
+      <c r="DV4" s="1" t="s">
+        <v>578</v>
+      </c>
       <c r="DW4" s="1" t="s">
         <v>404</v>
       </c>
@@ -4383,13 +4377,13 @@
         <v>201</v>
       </c>
       <c r="EX4" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="EY4" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="EZ4" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="FD4" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4688,7 +4682,7 @@
         <v>182</v>
       </c>
       <c r="DW5" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="DZ5" s="1">
         <f t="shared" si="2"/>
@@ -5067,7 +5061,7 @@
         <v>182</v>
       </c>
       <c r="DW6" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="DZ6" s="1">
         <f t="shared" si="2"/>
@@ -5432,10 +5426,7 @@
         <v>182</v>
       </c>
       <c r="DW7" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="DX7" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="DZ7" s="1">
         <f t="shared" si="2"/>
@@ -5506,13 +5497,13 @@
         <v>201</v>
       </c>
       <c r="EX7" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="EY7" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="EZ7" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="FD7" s="1" t="str">
         <f t="shared" si="10"/>
@@ -5832,15 +5823,12 @@
         <v>182</v>
       </c>
       <c r="DT8" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="DU8" s="1" t="s">
         <v>202</v>
       </c>
       <c r="DW8" s="1" t="s">
-        <v>571</v>
-      </c>
-      <c r="DX8" s="1" t="s">
         <v>569</v>
       </c>
       <c r="DZ8" s="1">
@@ -6229,13 +6217,10 @@
         <v>182</v>
       </c>
       <c r="DW9" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="DX9" s="1" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="DY9" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="DZ9" s="1">
         <f t="shared" si="2"/>
@@ -6306,13 +6291,13 @@
         <v>201</v>
       </c>
       <c r="EX9" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="EY9" s="1" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="EZ9" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="FD9" s="1" t="str">
         <f t="shared" si="10"/>
@@ -6632,7 +6617,7 @@
         <v>182</v>
       </c>
       <c r="DW10" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="DZ10" s="1">
         <f t="shared" ref="DZ10" si="17">DG10/EF10</f>
@@ -6703,13 +6688,13 @@
         <v>201</v>
       </c>
       <c r="EX10" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="EY10" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="EZ10" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="FD10" s="1" t="str">
         <f t="shared" si="10"/>

</xml_diff>